<commit_message>
Axis names in graphs
</commit_message>
<xml_diff>
--- a/2. Suma de enteros base DOS/SD-MTDeterminista1Cvs2C.xlsx
+++ b/2. Suma de enteros base DOS/SD-MTDeterminista1Cvs2C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cabez\OneDrive\Documentos\Uni\4º Curso\2º Cuatri\Teoría Avanzada de la Computación\Practicas\Practica 2\Practica_MT_TAC\2. Suma de enteros base DOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56EA23E5-2AAF-47F0-BB08-2973E8D28693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8268FD4A-708A-4CDA-8553-C5F2CBFC7BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F9F779F-0B5B-4B52-81CD-964E4560136B}"/>
   </bookViews>
@@ -253,10 +253,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.1344925634295712E-2"/>
-          <c:y val="0.17171296296296298"/>
-          <c:w val="0.88254396325459317"/>
-          <c:h val="0.6714577865266842"/>
+          <c:x val="9.3440527658180311E-2"/>
+          <c:y val="0.1717128516761374"/>
+          <c:w val="0.88455985203424348"/>
+          <c:h val="0.63023128483217528"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -437,6 +437,59 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>TAMAÑO</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -482,6 +535,7 @@
       <c:valAx>
         <c:axId val="1118020576"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -500,6 +554,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>PASOS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.0041038888843471E-2"/>
+              <c:y val="0.41342177925169571"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -544,6 +659,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.436276214486363"/>
+          <c:y val="0.92124930266297356"/>
+          <c:w val="0.17935931289102811"/>
+          <c:h val="5.8094883375973225E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1173,10 +1298,10 @@
       <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1503,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A09BB4A-54DC-429E-B086-C294D4F51FFD}">
   <dimension ref="B2:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:L5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>